<commit_message>
Them file pc05132asm2, chinh editor.jsp, sua lai entity cho asm, cap nhat file dtb.xls
</commit_message>
<xml_diff>
--- a/TableDTB.xlsx
+++ b/TableDTB.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9288"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9288" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="82">
   <si>
     <t>id</t>
   </si>
@@ -109,13 +109,167 @@
   </si>
   <si>
     <t>TyreType</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>imgsrc</t>
+  </si>
+  <si>
+    <t>Tyre</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>buys</t>
+  </si>
+  <si>
+    <t>@Entity</t>
+  </si>
+  <si>
+    <t>Like</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>likeDate</t>
+  </si>
+  <si>
+    <t>userLike</t>
+  </si>
+  <si>
+    <t>productLike</t>
+  </si>
+  <si>
+    <t>likeShare</t>
+  </si>
+  <si>
+    <t>userShare</t>
+  </si>
+  <si>
+    <t>productShare</t>
+  </si>
+  <si>
+    <t>productImg</t>
+  </si>
+  <si>
+    <t>tyre</t>
+  </si>
+  <si>
+    <t>@ManyToOne</t>
+  </si>
+  <si>
+    <t>@Table(name = "products")</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>@Table(name = "images")</t>
+  </si>
+  <si>
+    <t>@Table(name = "userss")</t>
+  </si>
+  <si>
+    <t>@Table(name = "tyres")</t>
+  </si>
+  <si>
+    <t>@Table(name = "likes")</t>
+  </si>
+  <si>
+    <t>@Table(name = "shares")</t>
+  </si>
+  <si>
+    <t>List&lt;Product&gt;</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>@JoinColumn(name = "product_id_fk_img")</t>
+  </si>
+  <si>
+    <t>@OneToMany(mappedBy = "product_id_fk_img")</t>
+  </si>
+  <si>
+    <t>List&lt;Image&gt;</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>@JoinColumn(name = "user_id_fk_like")</t>
+  </si>
+  <si>
+    <t>@OneToMany(mappedBy = "user_id_fk_like")</t>
+  </si>
+  <si>
+    <t>@JoinColumn(name = "product_id_fk_like")</t>
+  </si>
+  <si>
+    <t>@JoinColumn(name = "user_id_fk_share")</t>
+  </si>
+  <si>
+    <t>@JoinColumn(name = "product_id_fk_share")</t>
+  </si>
+  <si>
+    <t>@OneToMany(mappedBy = "product_id_fk_like")</t>
+  </si>
+  <si>
+    <t>List&lt;Like&gt;</t>
+  </si>
+  <si>
+    <t>likes</t>
+  </si>
+  <si>
+    <t>@OneToMany(mappedBy = "product_id_fk_share")</t>
+  </si>
+  <si>
+    <t>List&lt;Share&gt;</t>
+  </si>
+  <si>
+    <t>shares</t>
+  </si>
+  <si>
+    <t>@OneToMany(mappedBy = "user_id_fk_share")</t>
+  </si>
+  <si>
+    <t>@Id
+id</t>
+  </si>
+  <si>
+    <t>@OneToMany(mappedBy = "tyre_id_fk_product")</t>
+  </si>
+  <si>
+    <t>@JoinColumn(name = "tyre_id_fk_product")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,16 +277,93 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -140,12 +371,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,13 +1055,478 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.21875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.21875" customWidth="1"/>
+    <col min="8" max="8" width="1.21875" customWidth="1"/>
+    <col min="9" max="9" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="E1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="I1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="E2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="I2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="E3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="I3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="35"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="E10" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1"/>
+      <c r="I12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="E13" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="I13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E16" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="I16" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="25"/>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="I19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="I21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="5:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I22" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="I23" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="I24" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="27"/>
+    </row>
+    <row r="25" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="I25" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="J25" s="33"/>
+    </row>
+    <row r="26" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="I26" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="I27" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="27"/>
+    </row>
+    <row r="28" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="I28" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="J28" s="33"/>
+    </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="I29" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="I32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I33" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I34" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="9:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I37" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I38" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="J38" s="31"/>
+    </row>
+    <row r="39" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I40" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I41" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="J41" s="31"/>
+    </row>
+    <row r="42" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E13:F13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>